<commit_message>
Using pyannote speaker embeddings
</commit_message>
<xml_diff>
--- a/testing-results.xlsx
+++ b/testing-results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,60 +464,1336 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.01718313809728256</v>
+        <v>0.4418959072345788</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0405785382512448</v>
+        <v>0.7335480496377166</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03829921562550088</v>
+        <v>0.8929905166594549</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03697876259241925</v>
+        <v>0.9820916828526094</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03691871410409651</v>
+        <v>0.8537640662219894</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0388369981019116</v>
+        <v>0.8969473045780361</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03220566632313532</v>
+        <v>0.8212466888325278</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03128482267402617</v>
+        <v>0.9594567030011396</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01793238021713776</v>
+        <v>0.9186201205941359</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.03844285962107072</v>
+        <v>0.5209087269513447</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04842225776480812</v>
+        <v>0.8518894236831479</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02554842119901641</v>
+        <v>0.8891451282315986</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05325240484916312</v>
+        <v>0.9863086749905947</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04571872157609629</v>
+        <v>0.8835948767885888</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04759649097335862</v>
+        <v>0.9407172157262889</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0500471637658491</v>
+        <v>0.9420771217733107</v>
       </c>
       <c r="H3" t="n">
-        <v>0.04847674253126863</v>
+        <v>0.9059685938962264</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02720484961485034</v>
+        <v>0.9376612434486922</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.4639910562998484</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8756700369057501</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8636647442727814</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.009129682621313</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9047196979108276</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9221752003689978</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9291007181829286</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9612687892355957</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9966436827602552</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.4600992810699983</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8425522941964344</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9814643475103129</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.014744415531201</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9401719039076233</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9205677958933346</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9175290275939055</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9594038624374835</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.009564581541471</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.4804183957800741</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.7655181481942552</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8873108318814744</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.976490797695684</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.845177284104993</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8616171728814255</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.8929700589521273</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9720681823179822</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.028712840579127</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.3896974526458907</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8027341519537841</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.867744142110733</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.011906619227583</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8919032969894067</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.930669616722924</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.8841692741723197</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9674470117508732</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.004089157974895</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.4846509491980153</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8066704669258117</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8967943863873378</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9582644548065038</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8745813025088189</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9548212207646065</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.004088650532313</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9833560760070298</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.9660305447153703</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.4004683732452416</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.7738558276859128</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.9147330251654082</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.036948764283295</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.9480811006342128</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.944871800644718</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9066854506813505</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9501716829926472</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9633453378113571</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.543034044858836</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8121288108044148</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8929502660710205</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9926780536861773</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9424892600690914</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.929416870649886</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9357034735617125</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.000721971390285</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.024368844500565</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.411416021451097</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8403793935127868</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8686564069827546</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.022395523102039</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.8611637719351453</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.8846503828373218</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9363679847032903</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9725100407127236</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9404743822937838</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.6117546377113805</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8290692589638544</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.04418556885561</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9704907112590507</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8504167993728615</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9967748826382633</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9320503651978355</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9418999601538682</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.9026826023278915</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.5020978774447739</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.7929691865748335</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9771943713473208</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9991359095941422</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8909116034314989</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.9898397239618629</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.890407910996963</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9901311025334479</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.9378722723432539</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.8842967941274307</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.8918285395525921</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.3874247629970633</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.0390739287951</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.048330190955638</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9788937780312947</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.008828249954396</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9004420190980871</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.020017316479613</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.9164210042149211</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8777709335908432</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.4515065615054487</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.851905506070485</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8502228812886077</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.8808802938666789</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.8592562496667113</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.907162225645437</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.084609484535529</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.018780275996348</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.066948814145516</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.9812153465324608</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.9405551860538274</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.9854738961735174</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.8236078430770394</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8197764220196831</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.88628419453243</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.2498913831275326</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.9840432350950521</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.103257792820037</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.093368310414263</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.003430438500295</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.002455869390214</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9201786095909481</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8896034765422326</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8868419147352529</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2019981778725601</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.019642460457639</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1.038046097567871</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.030145789032433</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.9875689425757369</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.977598448320952</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.86234279230788</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.7992750231558068</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9521191840178845</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1959997067795963</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.9943284108424731</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.017839102128163</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.051023778682233</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.022322185978887</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.9408009889936525</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.8339475562855092</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.7486864314384578</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9365272837372712</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.2103591890272301</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.9694233798078508</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.010451241163203</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9470600598860525</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.044705126597333</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.8992977932198088</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.8725740709216152</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.7295518940406109</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.8999893372585059</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2366702092195182</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.018106745989932</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.029617214520135</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.020030283577029</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.042494872991395</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.9587599062365368</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.7885910658643029</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.7655126963672968</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.8800248825980603</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2416496650094695</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.9644134585248492</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.9990085788989916</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.07278333529001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.002074072975627</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.8996995824875911</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.7830967340519785</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.7751377942436588</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.9125762977839621</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.1969900557499291</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.9683601671530857</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.085506375572161</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.9556394369867417</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.020353342020272</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.9621940207000558</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.8658304547432616</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.7436103517791302</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9502426729530585</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.2305594122682793</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.9314151538576327</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.026618505067285</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.038093928159645</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.004496957387815</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9195064372002997</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.7963453015688154</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.8177207950411106</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.9154848835197275</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.1294746043613262</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.9663495305351915</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.064822190534723</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.051755622220719</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.02797887963327</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9044054007160253</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.909156478804438</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.8501000632435303</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.8443836569490899</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.1333705949647577</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1.090501338120809</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9985102681796691</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1.032933856870045</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.023378210429841</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9911561061701945</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.8008106995410551</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.9898960339512299</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.2681406468328381</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.8753698395894494</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1.073605011402897</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.012082679456249</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.06230696561028</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.9281535961313029</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.9607262804788247</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.7044668988479954</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.9243132043668846</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.2725038205459663</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8641546521144374</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.9656686327541409</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.9947357080403729</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.063952523144815</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.9377237781426829</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.9902398410329388</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.7841847431598838</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.9011194888176037</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.2603206933266328</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8713007012047613</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1.031297337898996</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.040609863641323</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1.043323104277008</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.9340959035519195</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.9204424286276527</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.7123875777607905</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.9606445048641703</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.241384480472624</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.8438846787863008</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1.049881762905462</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.024886885565798</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.028092005214216</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.9234275112556087</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.9282851811476489</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.7595581438919178</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.9400948018437465</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.3310297607534129</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.8535112729690194</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1.060110437001545</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.036637011497812</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.9612225639792308</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.981295890840447</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.9955774440266734</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.8004967856870262</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.9259736466462922</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.2464686743217803</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.8712659691991121</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.058349910009172</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.9826488479774448</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.027142692600227</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.9606411157183259</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.9064562736398099</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.7643497716002767</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.9279000818847237</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.2545945595297606</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.802937831139837</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1.030598890818708</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.034843756807222</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1.099811618408326</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.9981155619336699</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.904666448418334</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.6873695117248402</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.9033033314725974</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.3350886139024747</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.830797781263627</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1.077963466660985</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1.063996105946901</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1.055653362111118</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.02103092834698</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.9116279536605119</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.7461021319476202</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.9150106036418045</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.3275181825137377</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.8109646154997781</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1.011768933723405</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.048139912569749</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1.009998942416343</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.991510660446096</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.8549486358445217</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.7559032429271729</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.9754110373619468</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.2842150865456305</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.8676074948363218</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1.033880723361766</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.036113922803545</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.051974458363432</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.9315762671897979</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.954955665676898</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.8538726345462764</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.9577639241563811</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.2940962456182089</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.8238862346958866</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.9516593860719145</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.9308262268959226</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.8469101181431394</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.9477159942589344</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.8695650468218854</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.8340846775021853</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.202339772168365</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1.025323482472559</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.8215943959195783</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.9893137919544708</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.9227763288980043</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.8338668047119101</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.8915530202152295</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.887592944613153</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.919205546822716</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.2452397261309242</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.026463046259159</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.8785582997559234</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.9483060025198051</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.9901821193347545</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.9713609759925893</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.9153483771152978</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.9349963255087935</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.8508329379548452</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.1781730165578246</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.025023070245002</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.7816286692430178</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.9391915713680663</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.9531984981253998</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.8875607363592933</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.9468615320524222</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9590040906376753</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.9075854506551088</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.2230405739267121</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1.046701520335986</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.7605886310674164</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.9618570122068488</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.9873536560963003</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.8722258532632339</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.8944169408921103</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.8475955446972203</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.7947949045590905</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.2120245565387072</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1.007487977334234</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.7675306215281019</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.9694294636313534</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.9511786371670333</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.9438839822179962</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.914659710650879</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.8510637343858214</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.8478838063286445</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.2238576126084602</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1.101882357684254</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.7726112941422785</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.9486709900051568</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.8924332144537653</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.9231103658699802</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9594001948558035</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.8855159754640411</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.9234798877690519</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.2195001343371488</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.9892796093890268</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.8284080326252664</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.94054521635569</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.9352114092945499</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.9564372457261056</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.8939067129403052</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.8747571556619357</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.8602405521573491</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.2207119863817478</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.035900926055088</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.8119070004001483</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.9263017187050936</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.953902555536791</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.973034689614703</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.8986531961475075</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.9580752755032497</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.9325626581621623</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2020706582052937</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1.022242725872079</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.8308229883315272</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.9567700285516018</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.9410004247815971</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.9614398552785977</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9393136131841532</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.9682462210766145</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.942158371102209</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.179920684483667</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1.049372309113345</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.8225426216634348</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.906894044298317</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.9939578401278892</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.9820136609131305</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.9150161818531052</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.9204892238262258</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.893992645163155</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.1980531510277649</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1.085625520341123</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.7946609972275205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>